<commit_message>
supporting text or CSV file as input.
</commit_message>
<xml_diff>
--- a/src/Output/transcript_domains_DE.xlsx
+++ b/src/Output/transcript_domains_DE.xlsx
@@ -7,17 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Domains" sheetId="1" r:id="rId1"/>
+    <sheet name="ENST00000257910" sheetId="1" r:id="rId1"/>
+    <sheet name="ENST00000366578" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Transcript_ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="36">
   <si>
     <t>UniProt_ID</t>
   </si>
@@ -34,49 +32,97 @@
     <t>UniProt_URL</t>
   </si>
   <si>
-    <t>Domains</t>
-  </si>
-  <si>
-    <t>ENST00000257910</t>
-  </si>
-  <si>
-    <t>ENST00000366578</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
   <si>
     <t>Q12999</t>
   </si>
   <si>
+    <t>ENSG00000135452</t>
+  </si>
+  <si>
+    <t>TSPAN31</t>
+  </si>
+  <si>
+    <t>ENSP00000257910</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprotkb/Q12999/entry</t>
+  </si>
+  <si>
+    <t>Topological domain</t>
+  </si>
+  <si>
+    <t>Transmembrane</t>
+  </si>
+  <si>
+    <t>Cytoplasmic</t>
+  </si>
+  <si>
+    <t>Helical</t>
+  </si>
+  <si>
+    <t>Extracellular</t>
+  </si>
+  <si>
     <t>P35609</t>
   </si>
   <si>
-    <t>ENSG00000135452</t>
-  </si>
-  <si>
     <t>ENSG00000077522</t>
   </si>
   <si>
-    <t>TSPAN31</t>
-  </si>
-  <si>
     <t>ACTN2</t>
   </si>
   <si>
-    <t>ENSP00000257910</t>
-  </si>
-  <si>
     <t>ENSP00000355537</t>
   </si>
   <si>
-    <t>https://www.uniprot.org/uniprotkb/Q12999/entry</t>
-  </si>
-  <si>
     <t>https://www.uniprot.org/uniprotkb/P35609/entry</t>
   </si>
   <si>
-    <t>type:Topological domain,start:1,end:12,description:Cytoplasmic|type:Transmembrane,start:13,end:33,description:Helical|type:Topological domain,start:34,end:44,description:Extracellular|type:Transmembrane,start:45,end:65,description:Helical|type:Topological domain,start:66,end:72,description:Cytoplasmic|type:Transmembrane,start:73,end:93,description:Helical|type:Topological domain,start:94,end:173,description:Extracellular|type:Transmembrane,start:174,end:194,description:Helical|type:Topological domain,start:195,end:210,description:Cytoplasmic</t>
-  </si>
-  <si>
-    <t>type:Domain,start:38,end:142,description:Calponin-homology (CH) 1|type:Domain,start:151,end:257,description:Calponin-homology (CH) 2|type:Repeat,start:281,end:391,description:Spectrin 1|type:Repeat,start:401,end:506,description:Spectrin 2|type:Repeat,start:516,end:627,description:Spectrin 3|type:Repeat,start:637,end:740,description:Spectrin 4|type:Domain,start:753,end:788,description:EF-hand 1|type:Domain,start:789,end:824,description:EF-hand 2|type:Region,start:1,end:254,description:Actin-binding</t>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Calponin-homology (CH) 1</t>
+  </si>
+  <si>
+    <t>Calponin-homology (CH) 2</t>
+  </si>
+  <si>
+    <t>Spectrin 1</t>
+  </si>
+  <si>
+    <t>Spectrin 2</t>
+  </si>
+  <si>
+    <t>Spectrin 3</t>
+  </si>
+  <si>
+    <t>Spectrin 4</t>
+  </si>
+  <si>
+    <t>EF-hand 1</t>
+  </si>
+  <si>
+    <t>EF-hand 2</t>
+  </si>
+  <si>
+    <t>Actin-binding</t>
   </si>
 </sst>
 </file>
@@ -447,22 +493,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="48.7109375" customWidth="1"/>
-    <col min="7" max="7" width="549.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,57 +532,610 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G4">
+        <v>34</v>
+      </c>
+      <c r="H4">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>45</v>
+      </c>
+      <c r="H5">
+        <v>65</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>66</v>
+      </c>
+      <c r="H6">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>73</v>
+      </c>
+      <c r="H7">
+        <v>93</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>94</v>
+      </c>
+      <c r="H8">
+        <v>173</v>
+      </c>
+      <c r="I8" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>174</v>
+      </c>
+      <c r="H9">
+        <v>194</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>195</v>
+      </c>
+      <c r="H10">
+        <v>210</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>38</v>
+      </c>
+      <c r="H2">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>151</v>
+      </c>
+      <c r="H3">
+        <v>257</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>281</v>
+      </c>
+      <c r="H4">
+        <v>391</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>401</v>
+      </c>
+      <c r="H5">
+        <v>506</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>516</v>
+      </c>
+      <c r="H6">
+        <v>627</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>637</v>
+      </c>
+      <c r="H7">
+        <v>740</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>753</v>
+      </c>
+      <c r="H8">
+        <v>788</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>789</v>
+      </c>
+      <c r="H9">
+        <v>824</v>
+      </c>
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>254</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>